<commit_message>
fix stat hyperlink #9
</commit_message>
<xml_diff>
--- a/helpful/VisioTemplates_Stats.xlsx
+++ b/helpful/VisioTemplates_Stats.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E1C9B3-45AA-4D67-A86A-06CBEA7AE6F5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908FB860-2BA1-47A0-8F50-36ECF9E1E258}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1832,7 +1832,7 @@
   <dimension ref="A1:Q157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6928,162 +6928,162 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{E96C683E-B503-4969-8739-556F94CAC69F}"/>
-    <hyperlink ref="A3" r:id="rId2" display="../../../../../../Program Files (x86)/Microsoft Office/root/Office16/Visio Content/1049/ACTUAL_FINISHDATES_GANTTCHART_M.VSTX" xr:uid="{961D2BB5-9680-4411-B69D-5F602D54A649}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{84102B40-ECDF-4DE9-AE88-FE2B7D356321}"/>
-    <hyperlink ref="A157" r:id="rId4" xr:uid="{67F3E2A2-ABAB-47EB-B6E0-B134BBD3FBBB}"/>
-    <hyperlink ref="A156" r:id="rId5" xr:uid="{F71203A9-901E-4084-BCA9-9BD536C17A25}"/>
-    <hyperlink ref="A155" r:id="rId6" xr:uid="{94A4091E-01BF-4A73-B798-0EA4E42D2AEA}"/>
-    <hyperlink ref="A154" r:id="rId7" xr:uid="{7ECD5417-F2DE-4014-8749-DCA068FB24DF}"/>
-    <hyperlink ref="A153" r:id="rId8" xr:uid="{3F370577-B676-48D6-9513-ACD9CB05C1BC}"/>
-    <hyperlink ref="A152" r:id="rId9" xr:uid="{62803163-678B-4B94-8979-C346404C4202}"/>
-    <hyperlink ref="A151" r:id="rId10" xr:uid="{6043FE91-DBFC-403E-9E4B-4CAE50DEC63E}"/>
-    <hyperlink ref="A150" r:id="rId11" xr:uid="{8FAAFEFC-C7AF-41CF-A473-1D1E8BF00465}"/>
-    <hyperlink ref="A149" r:id="rId12" xr:uid="{34F00F33-FF40-41D8-9209-B3013F0B4B51}"/>
-    <hyperlink ref="A148" r:id="rId13" xr:uid="{A8D8D57A-C542-4477-B857-4130CCBF2F41}"/>
-    <hyperlink ref="A147" r:id="rId14" xr:uid="{D948F96A-6502-4129-A2D1-4AA700667268}"/>
-    <hyperlink ref="A146" r:id="rId15" xr:uid="{3CFA9DB3-50D6-4AF5-B739-249A0F104C3B}"/>
-    <hyperlink ref="A145" r:id="rId16" xr:uid="{512FFBB8-1733-40D2-B7E2-7C3ED9231EC5}"/>
-    <hyperlink ref="A144" r:id="rId17" xr:uid="{BBB53011-E19F-40AA-BC9C-3E9F7D3917F6}"/>
-    <hyperlink ref="A143" r:id="rId18" xr:uid="{0126013D-A58E-4107-A40D-921E2BAA5BF2}"/>
-    <hyperlink ref="A142" r:id="rId19" xr:uid="{A733F893-04ED-444A-AE71-1A1E2BCA3C80}"/>
-    <hyperlink ref="A141" r:id="rId20" xr:uid="{A86C56C5-BBF3-4CB1-A8C5-EFA8BC624495}"/>
-    <hyperlink ref="A140" r:id="rId21" xr:uid="{1D024248-EF36-48E0-97F7-CAB112B5645F}"/>
-    <hyperlink ref="A139" r:id="rId22" xr:uid="{018A28FA-5A87-41FE-87DE-C79A8AABDCD0}"/>
-    <hyperlink ref="A138" r:id="rId23" xr:uid="{DC0F2AF8-9A4A-4A3E-A3C5-FAA54089AC8E}"/>
-    <hyperlink ref="A137" r:id="rId24" xr:uid="{B63BF417-C8B9-43F2-A48F-D5C63E719D80}"/>
-    <hyperlink ref="A136" r:id="rId25" xr:uid="{FB735693-E218-4C57-ABBB-21A64DC84043}"/>
-    <hyperlink ref="A135" r:id="rId26" xr:uid="{876C9555-1825-4DD3-A866-01F81A051CDE}"/>
-    <hyperlink ref="A134" r:id="rId27" xr:uid="{13122E35-B6EF-4D9B-8E0E-CA6388840F89}"/>
-    <hyperlink ref="A133" r:id="rId28" xr:uid="{C47C8099-C020-4259-9E85-83261934C0E3}"/>
-    <hyperlink ref="A132" r:id="rId29" xr:uid="{8353C8C2-BC57-4408-9A5D-7A6C5593CC10}"/>
-    <hyperlink ref="A131" r:id="rId30" xr:uid="{44C29E09-957E-4374-B21C-21A12429C20F}"/>
-    <hyperlink ref="A130" r:id="rId31" xr:uid="{B8A1ACA6-A1B4-40D4-806A-9CB058BDE34B}"/>
-    <hyperlink ref="A129" r:id="rId32" xr:uid="{A6EF404C-5B4A-4237-89D6-DA4999099953}"/>
-    <hyperlink ref="A128" r:id="rId33" xr:uid="{5940A4B5-5EB2-42F9-B460-93729F0378F2}"/>
-    <hyperlink ref="A127" r:id="rId34" xr:uid="{AEDE7845-46EC-4FC7-90FF-7EE7A82F32F6}"/>
-    <hyperlink ref="A126" r:id="rId35" xr:uid="{6B933CD0-ABE7-4AAE-ADE2-121EF2E50985}"/>
-    <hyperlink ref="A125" r:id="rId36" xr:uid="{EE494F00-9752-4486-B0C8-543770579DCB}"/>
-    <hyperlink ref="A124" r:id="rId37" xr:uid="{E28069AD-284B-4907-805A-DADF2FE18E87}"/>
-    <hyperlink ref="A123" r:id="rId38" xr:uid="{F1DA669A-E5EE-4EF4-8041-C52D34B455E3}"/>
-    <hyperlink ref="A122" r:id="rId39" xr:uid="{631016DD-E68E-4598-B663-22AB50AAFE77}"/>
-    <hyperlink ref="A121" r:id="rId40" xr:uid="{83636BF9-3DAE-4DDA-B8AB-8B1DDAADB1F8}"/>
-    <hyperlink ref="A120" r:id="rId41" xr:uid="{DC989A4F-78D6-4FFC-A095-151085223571}"/>
-    <hyperlink ref="A119" r:id="rId42" xr:uid="{2B599E00-8EBE-4F26-8311-9D58EEB53872}"/>
-    <hyperlink ref="A118" r:id="rId43" xr:uid="{11DC71F5-1F72-403E-B7D6-E6A93ED8ABC3}"/>
-    <hyperlink ref="A117" r:id="rId44" xr:uid="{E0938645-C604-4E7A-9AFA-783EB3AC97E3}"/>
-    <hyperlink ref="A116" r:id="rId45" xr:uid="{8B88C953-446E-4CC3-8589-2D41B03364A0}"/>
-    <hyperlink ref="A115" r:id="rId46" xr:uid="{200E838D-F8A4-41CB-A580-AFE97CA48859}"/>
-    <hyperlink ref="A114" r:id="rId47" xr:uid="{B607BEF5-EBAC-4632-A639-304CC11EBD26}"/>
-    <hyperlink ref="A113" r:id="rId48" xr:uid="{6999D4BD-9472-4234-80C4-91C8462847D3}"/>
-    <hyperlink ref="A112" r:id="rId49" xr:uid="{5476EF90-84CE-4AA7-A43D-E9E7A0DE1710}"/>
-    <hyperlink ref="A111" r:id="rId50" xr:uid="{292BE876-5B30-48EE-8F48-3871BAB005E0}"/>
-    <hyperlink ref="A110" r:id="rId51" xr:uid="{74D4FDA3-B040-4252-95A1-FC941A6CE935}"/>
-    <hyperlink ref="A109" r:id="rId52" xr:uid="{7984C13D-B908-4102-992B-204BA58C26F8}"/>
-    <hyperlink ref="A108" r:id="rId53" xr:uid="{A55CE6EA-2769-4DF4-8BD1-A38E76B4C6C0}"/>
-    <hyperlink ref="A107" r:id="rId54" xr:uid="{254D1092-5B27-4A41-976E-2F2C8864ED1F}"/>
-    <hyperlink ref="A106" r:id="rId55" xr:uid="{5A15CBBC-CABD-43D2-A94B-6427C8798416}"/>
-    <hyperlink ref="A105" r:id="rId56" xr:uid="{616E886F-293B-4B7B-BD5B-78D8DAC135F3}"/>
-    <hyperlink ref="A104" r:id="rId57" xr:uid="{8D8E6CA3-F121-4FC2-BE3A-EB58A13045ED}"/>
-    <hyperlink ref="A103" r:id="rId58" xr:uid="{CE0EE683-B718-48DE-8D7C-F24C7726D7EC}"/>
-    <hyperlink ref="A102" r:id="rId59" xr:uid="{9A31257C-AB0A-45BD-861F-4B0C1D86B5D0}"/>
-    <hyperlink ref="A101" r:id="rId60" xr:uid="{F711B332-0BF2-4DD6-AA47-761EBB64E154}"/>
-    <hyperlink ref="A100" r:id="rId61" xr:uid="{E687A849-FFEC-41CE-A560-9D0CC688410E}"/>
-    <hyperlink ref="A99" r:id="rId62" xr:uid="{D3702FF4-4BAA-4006-A9BD-08BC2E3A5C5B}"/>
-    <hyperlink ref="A98" r:id="rId63" xr:uid="{6B1F1D5C-DA80-4E95-BB55-FE5C5CDE11E8}"/>
-    <hyperlink ref="A97" r:id="rId64" xr:uid="{6C8A32A9-6883-435B-B989-509F41378884}"/>
-    <hyperlink ref="A96" r:id="rId65" xr:uid="{232DA7A0-0ABC-46D7-8EE9-E34D769BD5B6}"/>
-    <hyperlink ref="A95" r:id="rId66" xr:uid="{086652A3-2FCA-4161-87B6-85F8B7D7E4B5}"/>
-    <hyperlink ref="A94" r:id="rId67" xr:uid="{E2C04223-7C7C-4636-9843-47FC834E1A4D}"/>
-    <hyperlink ref="A93" r:id="rId68" xr:uid="{62479076-7E99-4774-AB5B-1979CA1FDBB3}"/>
-    <hyperlink ref="A92" r:id="rId69" xr:uid="{BA419263-F5BB-4AA4-82E9-6B9A20512A58}"/>
-    <hyperlink ref="A91" r:id="rId70" xr:uid="{9AC1E0FD-E3F2-4945-9D60-F3B59403423F}"/>
-    <hyperlink ref="A90" r:id="rId71" xr:uid="{B34B86EE-37FD-42B2-892B-8A555D5C4AEC}"/>
-    <hyperlink ref="A89" r:id="rId72" xr:uid="{9DCC01E4-D5BF-42B1-A778-298E2F5504A2}"/>
-    <hyperlink ref="A88" r:id="rId73" xr:uid="{D42ACBDA-0A31-4049-9CB9-775F42F4C5CE}"/>
-    <hyperlink ref="A87" r:id="rId74" xr:uid="{B94D2ED4-E708-4AA1-A00F-F274B717D913}"/>
-    <hyperlink ref="A86" r:id="rId75" xr:uid="{8BDE6CB3-DE8D-4D62-B15A-24AE11E5C238}"/>
-    <hyperlink ref="A85" r:id="rId76" xr:uid="{F9200980-2D6F-4197-983C-AEEF37AF2946}"/>
-    <hyperlink ref="A84" r:id="rId77" xr:uid="{F964D9EC-44AE-4BE2-9103-1E2F10CF655D}"/>
-    <hyperlink ref="A83" r:id="rId78" xr:uid="{32A59004-2F29-4FB0-97F8-605D7F5A3883}"/>
-    <hyperlink ref="A82" r:id="rId79" xr:uid="{F768453B-BEF7-4D7F-8BFB-D58A03FEC10D}"/>
-    <hyperlink ref="A81" r:id="rId80" xr:uid="{AEBB523B-9E31-4FAB-B048-0A5686347FFC}"/>
-    <hyperlink ref="A80" r:id="rId81" xr:uid="{3B237AC2-9F81-4E9A-AEC0-DF60FE95B467}"/>
-    <hyperlink ref="A79" r:id="rId82" xr:uid="{3251A4EB-6FB8-4A2C-94D3-026117168B2C}"/>
-    <hyperlink ref="A78" r:id="rId83" xr:uid="{DB3F72DA-8AAD-4790-BA02-47E2A2EC00BF}"/>
-    <hyperlink ref="A77" r:id="rId84" xr:uid="{6263799D-EB4F-49B8-B1D5-948CCD149BB4}"/>
-    <hyperlink ref="A76" r:id="rId85" xr:uid="{1262146A-AF1E-45CF-9DE5-2B5A3E27421A}"/>
-    <hyperlink ref="A75" r:id="rId86" xr:uid="{BFAD318D-3190-4364-BA36-50AE38120E45}"/>
-    <hyperlink ref="A74" r:id="rId87" xr:uid="{A524F749-A97D-4384-A55E-5625903F0425}"/>
-    <hyperlink ref="A73" r:id="rId88" xr:uid="{ABC9C551-3E2E-4DED-B9EB-5C2329E7C7B0}"/>
-    <hyperlink ref="A72" r:id="rId89" xr:uid="{8783AFD0-F9EF-43FF-877B-14EB2594F780}"/>
-    <hyperlink ref="A71" r:id="rId90" xr:uid="{685F7FED-2D89-42A1-8431-2584A691B38F}"/>
-    <hyperlink ref="A70" r:id="rId91" xr:uid="{3EDB5B9D-2719-409E-8A39-C7AA39D1481F}"/>
-    <hyperlink ref="A69" r:id="rId92" xr:uid="{A2119EE1-933D-40DF-840A-2CC07A1CAAF3}"/>
-    <hyperlink ref="A68" r:id="rId93" xr:uid="{EC832652-9B12-4106-85C6-85F1139DC894}"/>
-    <hyperlink ref="A67" r:id="rId94" xr:uid="{4046D22A-4F42-4DFB-956E-88D51453FBB1}"/>
-    <hyperlink ref="A66" r:id="rId95" xr:uid="{3007DE6E-C1E1-4BD9-B5B3-B22DB40BB564}"/>
-    <hyperlink ref="A65" r:id="rId96" xr:uid="{541B2B56-E41C-4570-BC6C-50C377CF4AB5}"/>
-    <hyperlink ref="A64" r:id="rId97" xr:uid="{995E7008-F6B4-49E9-BA73-727EB78BAD3D}"/>
-    <hyperlink ref="A63" r:id="rId98" xr:uid="{0ED5327E-5FB6-4FF5-A5C8-A1F75BCFF6E7}"/>
-    <hyperlink ref="A62" r:id="rId99" xr:uid="{5A1D7BC0-B6E5-458E-A702-0BA716983054}"/>
-    <hyperlink ref="A61" r:id="rId100" xr:uid="{40490289-61DD-4107-9834-593EAC48FB77}"/>
-    <hyperlink ref="A60" r:id="rId101" xr:uid="{96AEE566-1EC7-4EDE-9B19-CDA72EBE728B}"/>
-    <hyperlink ref="A59" r:id="rId102" xr:uid="{36978FE6-9052-45A8-B37D-C937B28B0E1C}"/>
-    <hyperlink ref="A58" r:id="rId103" xr:uid="{064F350B-5ECE-40EF-8481-7F0DE57E65F5}"/>
-    <hyperlink ref="A57" r:id="rId104" xr:uid="{C1F79028-0804-4969-9241-F53CFE3807AB}"/>
-    <hyperlink ref="A56" r:id="rId105" xr:uid="{BC5F67FD-1F2B-4A0C-B3B5-AF76575669D4}"/>
-    <hyperlink ref="A55" r:id="rId106" xr:uid="{D4BD938F-3C00-4DEA-9632-9C34AE3C0712}"/>
-    <hyperlink ref="A54" r:id="rId107" xr:uid="{BB18CB29-A901-41E2-80BC-0EE0F0A883AC}"/>
-    <hyperlink ref="A53" r:id="rId108" xr:uid="{EB25A9EE-B343-4627-B202-38D4685F81FA}"/>
-    <hyperlink ref="A52" r:id="rId109" xr:uid="{15FAC4F1-A8E3-4583-AD62-9B1426FF92C3}"/>
-    <hyperlink ref="A51" r:id="rId110" xr:uid="{276F6FA9-A2D0-4FBF-8B80-DC26764A653A}"/>
-    <hyperlink ref="A50" r:id="rId111" xr:uid="{5364851C-F8A8-49CE-967C-5DEF7A378CC1}"/>
-    <hyperlink ref="A49" r:id="rId112" xr:uid="{FE73D752-E0BA-42DD-8568-495104EDF544}"/>
-    <hyperlink ref="A48" r:id="rId113" xr:uid="{183DF729-155D-40F2-874A-82B18914F6F1}"/>
-    <hyperlink ref="A47" r:id="rId114" xr:uid="{F6737AC2-76E8-451B-95D1-5D5699AFCF2F}"/>
-    <hyperlink ref="A46" r:id="rId115" xr:uid="{A9001197-D6DC-44D5-9CD2-61DA8D830D51}"/>
-    <hyperlink ref="A45" r:id="rId116" xr:uid="{45C56D22-ED62-4D45-8530-931F9FB5E957}"/>
-    <hyperlink ref="A44" r:id="rId117" xr:uid="{E5C2336B-B912-45BC-9628-94A796740BBF}"/>
-    <hyperlink ref="A43" r:id="rId118" xr:uid="{BBC75677-5ADC-4FCE-8D41-3DD018AC979A}"/>
-    <hyperlink ref="A42" r:id="rId119" xr:uid="{8E5801BA-3A5D-4BBB-B2CA-B68937CE1E19}"/>
-    <hyperlink ref="A41" r:id="rId120" xr:uid="{FDF2E6CE-4942-402F-944B-E9ECCB822EFC}"/>
-    <hyperlink ref="A40" r:id="rId121" xr:uid="{6408C319-8D4A-4C0A-8945-BD935F10EC67}"/>
-    <hyperlink ref="A39" r:id="rId122" xr:uid="{A7CDE216-C18A-4502-80F1-79FEA82E8FC0}"/>
-    <hyperlink ref="A38" r:id="rId123" xr:uid="{5A6C9DFF-C092-4EDB-B92E-9CA9876FD85F}"/>
-    <hyperlink ref="A37" r:id="rId124" xr:uid="{16FE51F7-D1EA-4A5B-AE06-B238AC3AADAF}"/>
-    <hyperlink ref="A36" r:id="rId125" xr:uid="{D17939EA-7075-4032-BBF7-10E36335D593}"/>
-    <hyperlink ref="A35" r:id="rId126" xr:uid="{16A163AC-BB60-4655-B0EE-C53E2391BD46}"/>
-    <hyperlink ref="A34" r:id="rId127" xr:uid="{5085B272-249D-44B1-8122-A610C283680E}"/>
-    <hyperlink ref="A33" r:id="rId128" xr:uid="{4B17809F-6E02-4B9B-B2B0-82F31623929D}"/>
-    <hyperlink ref="A32" r:id="rId129" xr:uid="{839EFA4A-D069-4E11-8FE8-46C7DE55D661}"/>
-    <hyperlink ref="A31" r:id="rId130" xr:uid="{33C29AF6-BCEF-4155-AD3D-BA95CEF37D75}"/>
-    <hyperlink ref="A30" r:id="rId131" xr:uid="{57DEAB2B-6691-45E5-AB9A-1B1F6186F68B}"/>
-    <hyperlink ref="A29" r:id="rId132" xr:uid="{ECBC4EEE-D70E-45E5-B8B8-23F74E5F4C6D}"/>
-    <hyperlink ref="A28" r:id="rId133" xr:uid="{EEF45C1F-C616-443C-B8E9-0CE286C1D36F}"/>
-    <hyperlink ref="A27" r:id="rId134" xr:uid="{DA9D18C6-ABCB-4263-9E4E-213FDDADA9EC}"/>
-    <hyperlink ref="A26" r:id="rId135" xr:uid="{6FD155D7-C180-4B19-8324-616F54DE0229}"/>
-    <hyperlink ref="A25" r:id="rId136" xr:uid="{396F1C48-724F-4261-92C6-E8CFE9BFAD1C}"/>
-    <hyperlink ref="A24" r:id="rId137" xr:uid="{67029E1C-E4D9-4DF2-B0B6-DED7F2B51D3D}"/>
-    <hyperlink ref="A23" r:id="rId138" xr:uid="{31228E63-6BD0-4168-B695-206FB4839601}"/>
-    <hyperlink ref="A22" r:id="rId139" xr:uid="{4EBF73C9-2DCD-46C9-8B85-F0D0A6455C1F}"/>
-    <hyperlink ref="A21" r:id="rId140" xr:uid="{F8DBF631-5914-48D2-82FE-60FB8EA5DBF2}"/>
-    <hyperlink ref="A20" r:id="rId141" xr:uid="{CBA7A981-80F3-4B51-A7BF-B80506639C4A}"/>
-    <hyperlink ref="A19" r:id="rId142" xr:uid="{624CDCAA-3BD3-4C56-9F58-1EFB7B531C26}"/>
-    <hyperlink ref="A18" r:id="rId143" xr:uid="{4BEECC4B-AAD1-4348-85A3-B1F1BB461EEA}"/>
-    <hyperlink ref="A17" r:id="rId144" xr:uid="{26C75F9A-A191-4D06-9BD3-0E73420E0E33}"/>
-    <hyperlink ref="A16" r:id="rId145" xr:uid="{31ABC24F-60CC-4342-95AE-6D1184CB80CB}"/>
-    <hyperlink ref="A15" r:id="rId146" xr:uid="{023B1E97-AD63-49D5-9586-7D2E322399C9}"/>
-    <hyperlink ref="A14" r:id="rId147" xr:uid="{E8550EE0-236A-479F-BF45-1CDC61A3175B}"/>
-    <hyperlink ref="A13" r:id="rId148" xr:uid="{360E969E-4E88-427F-9F61-C4589A58EFE8}"/>
-    <hyperlink ref="A12" r:id="rId149" xr:uid="{0D53E1D1-5873-4E0D-86FB-811751E3C5B3}"/>
-    <hyperlink ref="A11" r:id="rId150" xr:uid="{EAA2181A-D010-466D-8703-6BB0B5F13345}"/>
-    <hyperlink ref="A10" r:id="rId151" xr:uid="{E26494F5-3E34-4068-A279-17A6748142D5}"/>
-    <hyperlink ref="A9" r:id="rId152" xr:uid="{E148EF5C-4300-4F8A-AE64-BA64238D8C34}"/>
-    <hyperlink ref="A8" r:id="rId153" xr:uid="{1665DA95-4E8D-4581-A265-88C94527C10C}"/>
-    <hyperlink ref="A7" r:id="rId154" xr:uid="{28FF3E16-6DFB-4D15-BA3B-665E0A2A052E}"/>
-    <hyperlink ref="A6" r:id="rId155" xr:uid="{4D6EE1AD-AFF1-48A5-95A0-04928B3096C1}"/>
-    <hyperlink ref="A5" r:id="rId156" xr:uid="{F583B9BE-90BA-4C71-BB49-2F3AFAAF7155}"/>
+    <hyperlink ref="A2" r:id="rId1" display="ACTDIR_" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" display="../../../../../../Program Files (x86)/Microsoft Office/root/Office16/Visio Content/1049/ACTUAL_FINISHDATES_GANTTCHART_M.VSTX" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" display="c:\Program Files (x86)\Microsoft Office\root\Office16\Visio Content\1049\ASSOCIATIONS_UML_CLASS_M.vstx" xr:uid="{89D2DEC5-3697-4F69-863E-1125A8D98D0D}"/>
+    <hyperlink ref="A5" r:id="rId4" display="c:\Program Files (x86)\Microsoft Office\root\Office16\Visio Content\1049\AUDIT_M.vstx" xr:uid="{7B19601E-0290-49EB-9F39-2085FC1A68EF}"/>
+    <hyperlink ref="A6" r:id="rId5" location="AUDIT_SEVERAL_OUTCOMES_M" display="AUDIT_SEVERAL_OUTCOMES_M.vstx - AUDIT_SEVERAL_OUTCOMES_M" xr:uid="{CD3913EC-9E92-4211-A5A6-6BA5B5F4EF12}"/>
+    <hyperlink ref="A7" r:id="rId6" location="AUDIT_SUBPROCESS_M" display="AUDIT_SUBPROCESS_M.vstx - AUDIT_SUBPROCESS_M" xr:uid="{25B22561-8159-4082-82B8-5FB53C3E32B3}"/>
+    <hyperlink ref="A8" r:id="rId7" location="BASFLO_M" xr:uid="{5CDDCD25-43C5-4F54-B5C4-5B177B8E2485}"/>
+    <hyperlink ref="A9" r:id="rId8" location="BASICCIRCUIT_DIAGRAM_M" display="BASICCIRCUIT_DIAGRAM_M.vstx - BASICCIRCUIT_DIAGRAM_M" xr:uid="{D05FB118-A728-4AB5-95DE-62C204380876}"/>
+    <hyperlink ref="A10" r:id="rId9" location="BASICD_M" display="BASICD_M.vstx - BASICD_M" xr:uid="{85E8E744-B177-476C-9D13-298209681BAC}"/>
+    <hyperlink ref="A11" r:id="rId10" location="BASICELECTRICAL_DIAGRAM_M" display="BASICELECTRICAL_DIAGRAM_M.vstx - BASICELECTRICAL_DIAGRAM_M" xr:uid="{0D32A0FF-0BCD-4BC5-B564-8B009EAD2276}"/>
+    <hyperlink ref="A12" r:id="rId11" location="BASIC_AUDITDIAGRAM_M" display="BASIC_AUDITDIAGRAM_M.vstx - BASIC_AUDITDIAGRAM_M" xr:uid="{DDCCF4E5-D4A3-46D2-AC83-EF932BBDADAE}"/>
+    <hyperlink ref="A13" r:id="rId12" location="BASIC_GANTTCHART_M" display="BASIC_GANTTCHART_M.vstx - BASIC_GANTTCHART_M" xr:uid="{9239069A-33F3-4887-A1D4-41C84A941D06}"/>
+    <hyperlink ref="A14" r:id="rId13" location="BASIC_HOME_NETWORK_M" display="BASIC_HOME_NETWORK_M.vstx - BASIC_HOME_NETWORK_M" xr:uid="{9324EBE6-F802-4B94-BFDC-086687360DD2}"/>
+    <hyperlink ref="A15" r:id="rId14" location="BASIC_UMLSEQUENCE_M" display="BASIC_UMLSEQUENCE_M.vstx - BASIC_UMLSEQUENCE_M" xr:uid="{658FBC71-1809-4E99-A59C-6D6869FFC75D}"/>
+    <hyperlink ref="A16" r:id="rId15" location="BF_DATAVISUALIZER_M" display="BF_DATAVISUALIZER_M.vstx - BF_DATAVISUALIZER_M" xr:uid="{2EAACD63-7075-491E-B945-671A98730A98}"/>
+    <hyperlink ref="A17" r:id="rId16" location="BLOCKP_M" display="BLOCKP_M.vstx - BLOCKP_M" xr:uid="{51553BBB-8F72-4BA0-8284-C8C50DB9E0B4}"/>
+    <hyperlink ref="A18" r:id="rId17" location="BLOCK_M" display="BLOCK_M.vstx - BLOCK_M" xr:uid="{376485DA-895D-4A58-85D6-DE64E46AFA4C}"/>
+    <hyperlink ref="A19" r:id="rId18" location="BPMN_ADDRESS_CHANGE_PROCESS_M" display="BPMN_ADDRESS_CHANGE_PROCESS_M.vstx - BPMN_ADDRESS_CHANGE_PROCESS_M" xr:uid="{AAFC7813-B566-499E-9352-E57B893714D1}"/>
+    <hyperlink ref="A20" r:id="rId19" location="BPMN_M" display="BPMN_M.vstx - BPMN_M" xr:uid="{5754906B-0A40-4521-9E25-37CC3CDB47FE}"/>
+    <hyperlink ref="A21" r:id="rId20" location="BPMN_PROCESS_GATEWAY_M" display="BPMN_PROCESS_GATEWAY_M.vstx - BPMN_PROCESS_GATEWAY_M" xr:uid="{EC180276-7A30-48A5-A465-EE6E5C042E86}"/>
+    <hyperlink ref="A22" r:id="rId21" location="BPMN_PROCESS_MULTIPLE_ROLES_M" display="BPMN_PROCESS_MULTIPLE_ROLES_M.vstx - BPMN_PROCESS_MULTIPLE_ROLES_M" xr:uid="{18F078B0-326E-46D8-AE5F-19499C3F5C49}"/>
+    <hyperlink ref="A23" r:id="rId22" location="BSTORM_M" display="BSTORM_M.vstx - BSTORM_M" xr:uid="{588677CB-A2E7-4F81-B3C0-9DF022E79E03}"/>
+    <hyperlink ref="A24" r:id="rId23" location="CALNDR_M" display="CALNDR_M.vstx - CALNDR_M" xr:uid="{2CC6FAA8-DFE6-404E-A9B1-15317B1BDA40}"/>
+    <hyperlink ref="A25" r:id="rId24" location="CAUSEF_M" display="CAUSEF_M.vstx - CAUSEF_M" xr:uid="{6428CFE6-CC2D-4722-8D51-0DA213CC77B0}"/>
+    <hyperlink ref="A26" r:id="rId25" location="CEILPL_M" display="CEILPL_M.vstx - CEILPL_M" xr:uid="{B9D865EE-F20C-4228-A790-3BA183B2C8E6}"/>
+    <hyperlink ref="A27" r:id="rId26" location="CFF_DATAVISUALIZER_M" display="CFF_DATAVISUALIZER_M.vstx - CFF_DATAVISUALIZER_M" xr:uid="{44A44B3F-4F7C-4396-9212-697941744BE9}"/>
+    <hyperlink ref="A28" r:id="rId27" location="CFF_HORIZONTAL_M" display="CFF_HORIZONTAL_M.vstx - CFF_HORIZONTAL_M" xr:uid="{34C1D70A-4465-43B3-B9BC-6AE4E54E7146}"/>
+    <hyperlink ref="A29" r:id="rId28" location="CFF_SHAREDPROCESS_M" display="CFF_SHAREDPROCESS_M.vstx - CFF_SHAREDPROCESS_M" xr:uid="{01B36EC8-826B-4526-8286-B079F85568D1}"/>
+    <hyperlink ref="A30" r:id="rId29" location="CFF_VERTICAL_M" display="CFF_VERTICAL_M.vstx - CFF_VERTICAL_M" xr:uid="{BC1F26F1-8E22-40F8-B89A-080B31BA2D21}"/>
+    <hyperlink ref="A31" r:id="rId30" location="CHART_M" display="CHART_M.vstx - CHART_M" xr:uid="{2CC9DCDA-932A-4006-AC60-4AF35E7F8044}"/>
+    <hyperlink ref="A32" r:id="rId31" location="COMOLE_M" display="COMOLE_M.vstx - COMOLE_M" xr:uid="{EA972DE2-A614-4D68-A7D2-9C4914D251DF}"/>
+    <hyperlink ref="A33" r:id="rId32" location="CONLOG_M" display="CONLOG_M.vstx - CONLOG_M" xr:uid="{02CAA6A4-D6E1-4F92-9BCF-6CF416ADB9C2}"/>
+    <hyperlink ref="A34" r:id="rId33" location="DATFLO_M" display="DATFLO_M.vstx - DATFLO_M" xr:uid="{0E2EF032-F9B0-45E6-85E1-7896C840ABEC}"/>
+    <hyperlink ref="A35" r:id="rId34" location="DATMOD_M" display="DATMOD_M.vstx - DATMOD_M" xr:uid="{124D6672-9B1E-418D-80FA-0D8FBFD77092}"/>
+    <hyperlink ref="A36" r:id="rId35" location="DBCHEN_M" display="DBCHEN_M.vstx - DBCHEN_M" xr:uid="{775361C3-02D5-404B-9E6C-A09C3A3ED30F}"/>
+    <hyperlink ref="A37" r:id="rId36" location="DBCROW_M" display="DBCROW_M.vstx - DBCROW_M" xr:uid="{3DC4EB53-7131-405B-BEF1-7C08E6E35507}"/>
+    <hyperlink ref="A38" r:id="rId37" location="DBIDEF1X_M" display="DBIDEF1X_M.vstx - DBIDEF1X_M" xr:uid="{D47D302A-ACC2-4ACC-9B3E-3DFBD9F994DC}"/>
+    <hyperlink ref="A39" r:id="rId38" location="DBMODL_M" display="DBMODL_M.vstx - DBMODL_M" xr:uid="{488EF072-27AF-43AA-8A7F-80CF9684F301}"/>
+    <hyperlink ref="A40" r:id="rId39" location="DBUML_M" display="DBUML_M.vstx - DBUML_M" xr:uid="{2F1B664A-CBA2-4BCC-87CD-C1389D351FB9}"/>
+    <hyperlink ref="A41" r:id="rId40" location="DEPTORGCHART_M" display="DEPTORGCHART_M.vstx - DEPTORGCHART_M" xr:uid="{1CF0530E-A85D-441D-922D-92A0E733A712}"/>
+    <hyperlink ref="A42" r:id="rId41" location="DOCUMENT_APPROVAL_WORKFLOW_M" display="DOCUMENT_APPROVAL_WORKFLOW_M.vstx - DOCUMENT_APPROVAL_WORKFLOW_M" xr:uid="{45062C57-966C-431C-8535-A07679276C98}"/>
+    <hyperlink ref="A43" r:id="rId42" location="DRILLD_M" display="DRILLD_M.vstx - DRILLD_M" xr:uid="{24166B42-19BD-4853-91D0-E3220E425837}"/>
+    <hyperlink ref="A44" r:id="rId43" location="DTLNET_M" display="DTLNET_M.vstx - DTLNET_M" xr:uid="{58AAF57F-A3EA-499F-9ECD-B9E601D9F258}"/>
+    <hyperlink ref="A45" r:id="rId44" location="DTLNME_M" display="DTLNME_M.vstx - DTLNME_M" xr:uid="{7CEC8962-D455-4A1F-9B67-52A50E1C7219}"/>
+    <hyperlink ref="A46" r:id="rId45" location="DWGCNV_M" display="DWGCNV_M.vstx - DWGCNV_M" xr:uid="{C5FFFA8E-72C3-4236-B316-1D3ADC2EB62F}"/>
+    <hyperlink ref="A47" r:id="rId46" location="EDU_EECHIP_M" display="EDU_EECHIP_M.vstx - EDU_EECHIP_M" xr:uid="{F74E28D6-CA26-4F79-8F6A-8BDDC4336E8C}"/>
+    <hyperlink ref="A48" r:id="rId47" location="EECHIP_M" display="EECHIP_M.vstx - EECHIP_M" xr:uid="{1BFD2A85-1F03-4540-AB61-F2ED5B97A317}"/>
+    <hyperlink ref="A49" r:id="rId48" location="EEGENR_M" display="EEGENR_M.vstx - EEGENR_M" xr:uid="{E0C536DC-68FF-427C-B70A-6C6362BAF3F2}"/>
+    <hyperlink ref="A50" r:id="rId49" location="EEICS_M" display="EEICS_M.vstx - EEICS_M" xr:uid="{A846E889-4A1D-42D9-91FE-4FF107637EE0}"/>
+    <hyperlink ref="A51" r:id="rId50" location="EESYS_M" display="EESYS_M.vstx - EESYS_M" xr:uid="{D416EA5C-EC5D-40A0-A729-395A5F6E5464}"/>
+    <hyperlink ref="A52" r:id="rId51" location="ELETEL_M" display="ELETEL_M.vstx - ELETEL_M" xr:uid="{D035752D-FB60-4244-B4C4-D63D1665E1E3}"/>
+    <hyperlink ref="A53" r:id="rId52" location="ENTAPP_M" display="ENTAPP_M.vstx - ENTAPP_M" xr:uid="{8FF10EC5-FE88-41BE-8D09-C1C17A679D83}"/>
+    <hyperlink ref="A54" r:id="rId53" location="EPC_M" display="EPC_M.vstx - EPC_M" xr:uid="{6AD7B20D-8571-439C-A69C-2189369A5C9C}"/>
+    <hyperlink ref="A55" r:id="rId54" location="FAULT_M" display="FAULT_M.vstx - FAULT_M" xr:uid="{98A9FBC0-371F-4CB5-B1D2-DD16764624F4}"/>
+    <hyperlink ref="A56" r:id="rId55" location="FLRPLN_M" display="FLRPLN_M.vstx - FLRPLN_M" xr:uid="{8074C296-4B12-44CD-9485-1EF5434086EE}"/>
+    <hyperlink ref="A57" r:id="rId56" location="FPALL_M" display="FPALL_M.vstx - FPALL_M" xr:uid="{4F61317F-7EB9-40EC-8D02-1C5365AE42E8}"/>
+    <hyperlink ref="A58" r:id="rId57" location="GANTT_M" display="GANTT_M.vstx - GANTT_M" xr:uid="{C6360633-8955-45B6-A484-DA3E2B86B7D7}"/>
+    <hyperlink ref="A59" r:id="rId58" location="HIERARCHICALORGCHART_M" display="HIERARCHICALORGCHART_M.vstx - HIERARCHICALORGCHART_M" xr:uid="{876E5B57-66FD-4B34-8D26-CE2FB6FADADA}"/>
+    <hyperlink ref="A60" r:id="rId59" location="HOMPLN_M" display="HOMPLN_M.vstx - HOMPLN_M" xr:uid="{EC5D3B86-3BE7-4AF0-BB70-9584F01B727A}"/>
+    <hyperlink ref="A61" r:id="rId60" location="HVAC_M" display="HVAC_M.vstx - HVAC_M" xr:uid="{50EEB86C-770D-4699-B493-A00AD1BBB2CE}"/>
+    <hyperlink ref="A62" r:id="rId61" location="IDEF0_M" display="IDEF0_M.vstx - IDEF0_M" xr:uid="{688828C4-5B01-42C0-971B-B3EFA91DFC0E}"/>
+    <hyperlink ref="A63" r:id="rId62" location="INTERFACE_UML_CLASS_M" display="INTERFACE_UML_CLASS_M.vstx - INTERFACE_UML_CLASS_M" xr:uid="{EE20D291-283B-41CC-AA31-300F791E5F0A}"/>
+    <hyperlink ref="A64" r:id="rId63" location="ITIL_M" display="ITIL_M.vstx - ITIL_M" xr:uid="{7B14C309-6896-407E-982E-5EEC70177CA7}"/>
+    <hyperlink ref="A65" r:id="rId64" location="LDAPDR_M" display="LDAPDR_M.vstx - LDAPDR_M" xr:uid="{8CE40121-0A21-4E30-B913-A68D0BFE22EB}"/>
+    <hyperlink ref="A66" r:id="rId65" location="MAP3D_M" display="MAP3D_M.vstx - MAP3D_M" xr:uid="{06560E25-E088-427C-9BB4-087AE0407263}"/>
+    <hyperlink ref="A67" r:id="rId66" location="MAP_M" display="MAP_M.vstx - MAP_M" xr:uid="{1142E6AC-2911-41AD-9CAC-5D259B0FD0BD}"/>
+    <hyperlink ref="A68" r:id="rId67" location="MEALL_M" display="MEALL_M.vstx - MEALL_M" xr:uid="{A8DD462F-6A0C-405F-8518-7A9D4E3ECDE6}"/>
+    <hyperlink ref="A69" r:id="rId68" location="MEDIUMENTERPRISECORPNET_M" display="MEDIUMENTERPRISECORPNET_M.vstx - MEDIUMENTERPRISECORPNET_M" xr:uid="{9C964E0E-BC98-4A98-9070-172DE4283D28}"/>
+    <hyperlink ref="A70" r:id="rId69" location="MRKTDG_M" display="MRKTDG_M.vstx - MRKTDG_M" xr:uid="{B20F6335-18E0-4B5C-A877-9E6222790761}"/>
+    <hyperlink ref="A71" r:id="rId70" location="NETWME_M" display="NETWME_M.vstx - NETWME_M" xr:uid="{C16BF303-B286-483B-8551-9C9049FE6B31}"/>
+    <hyperlink ref="A72" r:id="rId71" location="NETW_M" display="NETW_M.vstx - NETW_M" xr:uid="{1E9B015C-6C52-4BC4-B89F-A124100F3900}"/>
+    <hyperlink ref="A73" r:id="rId72" location="OFFLYT_M" display="OFFLYT_M.vstx - OFFLYT_M" xr:uid="{292EDEC0-9A06-472B-9120-93BA89F7CD96}"/>
+    <hyperlink ref="A74" r:id="rId73" location="ONPAGEFLOWCHART_M" display="ONPAGEFLOWCHART_M.vstx - ONPAGEFLOWCHART_M" xr:uid="{2BA60194-117C-4365-9CD8-9FF9A9F321EF}"/>
+    <hyperlink ref="A75" r:id="rId74" location="ORGCH_M" display="ORGCH_M.vstx - ORGCH_M" xr:uid="{DB2BEF4B-487C-4EE8-BD3D-CCCFD8784647}"/>
+    <hyperlink ref="A76" r:id="rId75" location="ORGWIZ_M" display="ORGWIZ_M.vstx - ORGWIZ_M" xr:uid="{86AB3A14-D57E-4A7A-B3A7-9830116ADB5B}"/>
+    <hyperlink ref="A77" r:id="rId76" location="PBASLN_M" display="PBASLN_M.vstx - PBASLN_M" xr:uid="{A637FA4D-6580-49E6-B1BE-251E1FD14FC0}"/>
+    <hyperlink ref="A78" r:id="rId77" location="PBLANK_M" display="PBLANK_M.vstx - PBLANK_M" xr:uid="{3DD80CA3-03A5-4D46-ABFE-84D678674626}"/>
+    <hyperlink ref="A79" r:id="rId78" location="PCRTSK_M" display="PCRTSK_M.vstx - PCRTSK_M" xr:uid="{26C24F8E-0441-43A7-9048-ED6C80AF315C}"/>
+    <hyperlink ref="A80" r:id="rId79" location="PCSHFL_M" display="PCSHFL_M.vstx - PCSHFL_M" xr:uid="{E572326B-B619-41A0-8DDA-3980777213A8}"/>
+    <hyperlink ref="A81" r:id="rId80" location="PEDG_M" display="PEDG_M.vstx - PEDG_M" xr:uid="{2E2E5467-F896-43D7-9CC2-50C062EEA2E0}"/>
+    <hyperlink ref="A82" r:id="rId81" location="PEPIPE_M" display="PEPIPE_M.vstx - PEPIPE_M" xr:uid="{D2DB3E08-6CF3-472E-9FC9-15C5B6E67048}"/>
+    <hyperlink ref="A83" r:id="rId82" location="PERT_M" display="PERT_M.vstx - PERT_M" xr:uid="{DBD92ABF-8371-4F98-B895-677B892328A2}"/>
+    <hyperlink ref="A84" r:id="rId83" location="PLMPIP_M" display="PLMPIP_M.vstx - PLMPIP_M" xr:uid="{033DAD35-BDEA-4743-A9EC-17D638281088}"/>
+    <hyperlink ref="A85" r:id="rId84" location="PLTLYT_M" display="PLTLYT_M.vstx - PLTLYT_M" xr:uid="{AB867C08-03A2-48B6-8831-0887F670CF0D}"/>
+    <hyperlink ref="A86" r:id="rId85" location="PRSAVL_M" display="PRSAVL_M.vstx - PRSAVL_M" xr:uid="{44503C48-06B3-442C-BECC-8B580050B610}"/>
+    <hyperlink ref="A87" r:id="rId86" location="PRSSTS_M" display="PRSSTS_M.vstx - PRSSTS_M" xr:uid="{2883199F-DDB3-4309-90C8-D7CDA90872AE}"/>
+    <hyperlink ref="A88" r:id="rId87" location="PSTRCT_M" display="PSTRCT_M.vstx - PSTRCT_M" xr:uid="{830DBD89-5F42-4468-98D6-1173E604C9DC}"/>
+    <hyperlink ref="A89" r:id="rId88" location="PTSKST_M" display="PTSKST_M.vstx - PTSKST_M" xr:uid="{454B406B-27E9-4057-810D-4AB454D27482}"/>
+    <hyperlink ref="A90" r:id="rId89" location="RACK_M" display="RACK_M.vstx - RACK_M" xr:uid="{6A54CE8A-2E0E-4527-BCB3-F9081A50E489}"/>
+    <hyperlink ref="A91" r:id="rId90" location="SDL_M" display="SDL_M.vstx - SDL_M" xr:uid="{EE666434-E749-4D66-B1E3-0AD71874C4B6}"/>
+    <hyperlink ref="A92" r:id="rId91" location="SECACC_M" display="SECACC_M.vstx - SECACC_M" xr:uid="{9311FA09-20F8-4CCB-A5F4-ACBAABF3197F}"/>
+    <hyperlink ref="A93" r:id="rId92" location="SHAREPOINT_EXTRANETTOPOLOGY_M" display="SHAREPOINT_EXTRANETTOPOLOGY_M.vstx - SHAREPOINT_EXTRANETTOPOLOGY_M" xr:uid="{9E8416E0-E0FB-4FA3-9456-B34B1362ABB2}"/>
+    <hyperlink ref="A94" r:id="rId93" location="SIMPLE_WORKFLOW_M" display="SIMPLE_WORKFLOW_M.vstx - SIMPLE_WORKFLOW_M" xr:uid="{9BD10633-9D93-4030-B1C7-02C7638B3B59}"/>
+    <hyperlink ref="A95" r:id="rId94" location="SITPLN_M" display="SITPLN_M.vstx - SITPLN_M" xr:uid="{E49A8743-652F-4F5E-9E57-BAF0EA0CD756}"/>
+    <hyperlink ref="A96" r:id="rId95" location="SIXSIG_M" display="SIXSIG_M.vstx - SIXSIG_M" xr:uid="{42A662AB-5C8F-4898-875E-E51B634BA012}"/>
+    <hyperlink ref="A97" r:id="rId96" location="SMALLMEDIUM_BUSINESS_NETWORK_M" display="SMALLMEDIUM_BUSINESS_NETWORK_M.vstx - SMALLMEDIUM_BUSINESS_NETWORK_M" xr:uid="{FA93D0B6-FFB3-430A-8918-4C66654EB2D2}"/>
+    <hyperlink ref="A98" r:id="rId97" location="SPCPLN_M" display="SPCPLN_M.vstx - SPCPLN_M" xr:uid="{144133DB-7E29-476B-835D-C6368474C3C0}"/>
+    <hyperlink ref="A99" r:id="rId98" location="SPW2_M" display="SPW2_M.vstx - SPW2_M" xr:uid="{52717091-DE1D-4239-BAC7-6372C0495544}"/>
+    <hyperlink ref="A100" r:id="rId99" location="SPW_M" display="SPW_M.vstx - SPW_M" xr:uid="{EB77C7D8-1958-464F-86E3-C68D5A60CEE2}"/>
+    <hyperlink ref="A101" r:id="rId100" location="SUBPROCESSFLOWCHART_M" display="SUBPROCESSFLOWCHART_M.vstx - SUBPROCESSFLOWCHART_M" xr:uid="{06581FAA-0DEC-48F5-A903-13202638650C}"/>
+    <hyperlink ref="A102" r:id="rId101" location="SUBTASKS_GANTTCHART_M" display="SUBTASKS_GANTTCHART_M.vstx - SUBTASKS_GANTTCHART_M" xr:uid="{1EE40A9A-D33F-4473-818B-162BCF5AE86F}"/>
+    <hyperlink ref="A103" r:id="rId102" location="TIMELN_CYLINDRICAL_M" display="TIMELN_CYLINDRICAL_M.vstx - TIMELN_CYLINDRICAL_M" xr:uid="{96B5A724-3E5A-494C-950B-FABE04A6C57B}"/>
+    <hyperlink ref="A104" r:id="rId103" location="TIMELN_EXPANDEDBLOCK_M" display="TIMELN_EXPANDEDBLOCK_M.vstx - TIMELN_EXPANDEDBLOCK_M" xr:uid="{AED39BB2-6678-4310-9EC4-2F3F199B0171}"/>
+    <hyperlink ref="A105" r:id="rId104" location="TIMELN_M" display="TIMELN_M.vstx - TIMELN_M" xr:uid="{258D43CC-3D94-4F28-A034-F99CD6BCA916}"/>
+    <hyperlink ref="A106" r:id="rId105" location="TIMELN_VERTICALBLOCK_M" display="TIMELN_VERTICALBLOCK_M.vstx - TIMELN_VERTICALBLOCK_M" xr:uid="{982D0E24-A310-4048-89C9-8C88BFF1C6E8}"/>
+    <hyperlink ref="A107" r:id="rId106" location="TQM_M" display="TQM_M.vstx - TQM_M" xr:uid="{29614B5C-647E-4616-BA5A-E6B3D3F47237}"/>
+    <hyperlink ref="A108" r:id="rId107" location="UACTME_M" display="UACTME_M.vstx - UACTME_M" xr:uid="{4AB866C1-6CF7-4046-9F9C-938170BD96AE}"/>
+    <hyperlink ref="A109" r:id="rId108" location="UCMNME_BASIC_M" display="UCMNME_BASIC_M.vstx - UCMNME_BASIC_M" xr:uid="{1D97D9AC-A1CD-4627-A405-972CAB127E85}"/>
+    <hyperlink ref="A110" r:id="rId109" location="UCMNME_BASIC_R2L" display="UCMNME_BASIC_R2L.vstx - UCMNME_BASIC_R2L" xr:uid="{080B2A37-3C9D-4D6E-80A7-B33F50186C5D}"/>
+    <hyperlink ref="A111" r:id="rId110" location="UCMNME_M" display="UCMNME_M.vstx - UCMNME_M" xr:uid="{52317754-95E1-4D94-B339-B55ED4B7C44E}"/>
+    <hyperlink ref="A112" r:id="rId111" location="UCMNME_SEQUENCEEXPRESSION_1_M" display="UCMNME_SEQUENCEEXPRESSION_1_M.vstx - UCMNME_SEQUENCEEXPRESSION_1_M" xr:uid="{A5BED127-5588-46F0-871D-BB356EA5BE5D}"/>
+    <hyperlink ref="A113" r:id="rId112" location="UCMNME_SEQUENCEEXPRESSION_1_R2L" display="UCMNME_SEQUENCEEXPRESSION_1_R2L.vstx - UCMNME_SEQUENCEEXPRESSION_1_R2L" xr:uid="{3875997C-524E-42C9-9E1F-C912BBE64420}"/>
+    <hyperlink ref="A114" r:id="rId113" location="UCMNME_SEQUENCEEXPRESSION_2_M" display="UCMNME_SEQUENCEEXPRESSION_2_M.vstx - UCMNME_SEQUENCEEXPRESSION_2_M" xr:uid="{BD69F093-EE04-4E00-A9BC-E86DEC159BB9}"/>
+    <hyperlink ref="A115" r:id="rId114" location="UCMNME_SEQUENCEEXPRESSION_2_R2L" display="UCMNME_SEQUENCEEXPRESSION_2_R2L.vstx - UCMNME_SEQUENCEEXPRESSION_2_R2L" xr:uid="{818FC0BD-FE83-4399-9067-5EE850C7B8A7}"/>
+    <hyperlink ref="A116" r:id="rId115" location="UCOMME_BASIC_M" display="UCOMME_BASIC_M.vstx - UCOMME_BASIC_M" xr:uid="{528E2B0C-C2E2-49E3-B021-3DCBF0D3225A}"/>
+    <hyperlink ref="A117" r:id="rId116" location="UCOMME_BASIC_R2L" display="UCOMME_BASIC_R2L.vstx - UCOMME_BASIC_R2L" xr:uid="{AA0F0577-46AF-413D-AE6B-9F8E5047AE39}"/>
+    <hyperlink ref="A118" r:id="rId117" location="UCOMME_M" display="UCOMME_M.vstx - UCOMME_M" xr:uid="{46DC1C7B-BF0A-42C5-AD7D-2AF3E13643F7}"/>
+    <hyperlink ref="A119" r:id="rId118" location="UCOMME_MODULE_M" display="UCOMME_MODULE_M.vstx - UCOMME_MODULE_M" xr:uid="{8F36D56B-7A6E-4701-B2ED-FD469946459B}"/>
+    <hyperlink ref="A120" r:id="rId119" location="UCOMME_MODULE_R2L" display="UCOMME_MODULE_R2L.vstx - UCOMME_MODULE_R2L" xr:uid="{FE757AE3-84C0-401E-BB77-DD8B388E20FF}"/>
+    <hyperlink ref="A121" r:id="rId120" location="UCOMME_SUBSYSTEM_M" display="UCOMME_SUBSYSTEM_M.vstx - UCOMME_SUBSYSTEM_M" xr:uid="{62BBAAA0-9677-4C88-B4A4-94486729D18F}"/>
+    <hyperlink ref="A122" r:id="rId121" location="UCOMME_SUBSYSTEM_R2L" display="UCOMME_SUBSYSTEM_R2L.vstx - UCOMME_SUBSYSTEM_R2L" xr:uid="{134DC90E-1F0F-4EDE-B01F-A8AA34F0145A}"/>
+    <hyperlink ref="A123" r:id="rId122" location="UDEPME_BASIC_M" display="UDEPME_BASIC_M.vstx - UDEPME_BASIC_M" xr:uid="{1FB92DE8-46AE-4E6D-809F-F6EB8892519E}"/>
+    <hyperlink ref="A124" r:id="rId123" location="UDEPME_BASIC_R2L" display="UDEPME_BASIC_R2L.vstx - UDEPME_BASIC_R2L" xr:uid="{C24F3F98-B1B4-43B4-ABD4-16F24AA9CD58}"/>
+    <hyperlink ref="A125" r:id="rId124" location="UDEPME_HIERARCHICAL_NODES_M" display="UDEPME_HIERARCHICAL_NODES_M.vstx - UDEPME_HIERARCHICAL_NODES_M" xr:uid="{4B661701-1CAC-4477-9870-6668BB0A26E6}"/>
+    <hyperlink ref="A126" r:id="rId125" location="UDEPME_HIERARCHICAL_NODES_R2L" display="UDEPME_HIERARCHICAL_NODES_R2L.vstx - UDEPME_HIERARCHICAL_NODES_R2L" xr:uid="{011DD0EA-46D9-46C1-8302-0082560D0594}"/>
+    <hyperlink ref="A127" r:id="rId126" location="UDEPME_M" display="UDEPME_M.vstx - UDEPME_M" xr:uid="{49EEF167-A561-4FE3-BCB1-56A51528280E}"/>
+    <hyperlink ref="A128" r:id="rId127" location="UDEPME_MANIFESTATION_M" display="UDEPME_MANIFESTATION_M.vstx - UDEPME_MANIFESTATION_M" xr:uid="{30BE9C6D-5971-4C13-BC95-3DE33445FCFA}"/>
+    <hyperlink ref="A129" r:id="rId128" location="UDEPME_MANIFESTATION_R2L" display="UDEPME_MANIFESTATION_R2L.vstx - UDEPME_MANIFESTATION_R2L" xr:uid="{EFE9FE36-1896-4BB1-8206-80D2575EFDEA}"/>
+    <hyperlink ref="A130" r:id="rId129" location="UMLSEQUENCE_INTERACTIONFRAME_M" display="UMLSEQUENCE_INTERACTIONFRAME_M.vstx - UMLSEQUENCE_INTERACTIONFRAME_M" xr:uid="{18D97B31-3127-44A8-BB4D-75605AFE3475}"/>
+    <hyperlink ref="A131" r:id="rId130" location="UMLSEQUENCE_LOOP_M" display="UMLSEQUENCE_LOOP_M.vstx - UMLSEQUENCE_LOOP_M" xr:uid="{6C21402B-868D-47B6-971F-2D5C92964F3C}"/>
+    <hyperlink ref="A132" r:id="rId131" location="UML_CLASS_M" display="UML_CLASS_M.vstx - UML_CLASS_M" xr:uid="{FE112B84-6300-4424-BE64-A4738F2BBDCE}"/>
+    <hyperlink ref="A133" r:id="rId132" location="UML_USECASE_DEPENDENCIES_M" display="UML_USECASE_DEPENDENCIES_M.vstx - UML_USECASE_DEPENDENCIES_M" xr:uid="{52F369D4-D057-4D61-B293-1C4C30900681}"/>
+    <hyperlink ref="A134" r:id="rId133" location="UML_USECASE_M" display="UML_USECASE_M.vstx - UML_USECASE_M" xr:uid="{95D741C8-1A1B-4DFB-AFEF-01FA2AD87E71}"/>
+    <hyperlink ref="A135" r:id="rId134" location="UML_USECASE_SUBSYSTEM_M" display="UML_USECASE_SUBSYSTEM_M.vstx - UML_USECASE_SUBSYSTEM_M" xr:uid="{C2C0BEA2-E684-46C3-98C8-5AF06AA9EF86}"/>
+    <hyperlink ref="A136" r:id="rId135" location="USEQME_M" display="USEQME_M.vstx - USEQME_M" xr:uid="{E4808BFF-B90C-40F4-B03E-E5CA9A25357A}"/>
+    <hyperlink ref="A137" r:id="rId136" location="USTAME_M" display="USTAME_M.vstx - USTAME_M" xr:uid="{33A4F0BE-C29A-4B5B-B267-37BDA2CD85B2}"/>
+    <hyperlink ref="A138" r:id="rId137" location="USTRME_M" display="USTRME_M.vstx - USTRME_M" xr:uid="{8D8996A1-0C2A-4067-A70F-E8B0D34C2450}"/>
+    <hyperlink ref="A139" r:id="rId138" location="UUSEME_M" display="UUSEME_M.vstx - UUSEME_M" xr:uid="{476B402F-0655-4D59-A503-38909F01A8B5}"/>
+    <hyperlink ref="A140" r:id="rId139" location="VERTICALFLOWCHART_M" display="VERTICALFLOWCHART_M.vstx - VERTICALFLOWCHART_M" xr:uid="{AA10FEBA-E458-4ED4-9342-E9FF28398A4F}"/>
+    <hyperlink ref="A141" r:id="rId140" location="VSM_M" display="VSM_M.vstx - VSM_M" xr:uid="{7A16C1DF-C7C9-4E6B-BEBE-785897482FF5}"/>
+    <hyperlink ref="A142" r:id="rId141" location="WEBMAP_M" display="WEBMAP_M.vstx - WEBMAP_M" xr:uid="{FEA76742-775C-4470-98F0-CA11DA744953}"/>
+    <hyperlink ref="A143" r:id="rId142" location="WEBSIT_M" display="WEBSIT_M.vstx - WEBSIT_M" xr:uid="{EEC43178-1BFD-4741-801D-623EE680B5CA}"/>
+    <hyperlink ref="A144" r:id="rId143" location="WFDGM_M" display="WFDGM_M.vstx - WFDGM_M" xr:uid="{80928EDA-05AD-4986-A95D-7A15C8CD74A8}"/>
+    <hyperlink ref="A145" r:id="rId144" location="WORKFLOW_DEPARTMENTAL_M" display="WORKFLOW_DEPARTMENTAL_M.vstx - WORKFLOW_DEPARTMENTAL_M" xr:uid="{93803FE4-343A-42C9-8BAE-2B5D2477349E}"/>
+    <hyperlink ref="A146" r:id="rId145" location="WORKFLOW_FUNCTION_M" display="WORKFLOW_FUNCTION_M.vstx - WORKFLOW_FUNCTION_M" xr:uid="{6BBB2D46-C3B7-4B36-9FB9-8D9D507358C9}"/>
+    <hyperlink ref="A147" r:id="rId146" location="WORKFLOW_PROCESS_M" display="WORKFLOW_PROCESS_M.vstx - WORKFLOW_PROCESS_M" xr:uid="{78C0235E-42F2-4F71-9D4F-7CF6DB977641}"/>
+    <hyperlink ref="A148" r:id="rId147" location="WRKFLO_M" display="WRKFLO_M.vstx - WRKFLO_M" xr:uid="{4A104CF2-432C-43FA-8077-8E5EFAD86916}"/>
+    <hyperlink ref="A149" r:id="rId148" location="WRKFME_M" display="WRKFME_M.vstx - WRKFME_M" xr:uid="{77EE55C9-1E04-4BDA-9971-98E62DD4D39E}"/>
+    <hyperlink ref="A150" r:id="rId149" location="WWFC_BLOG_M" display="WWFC_BLOG_M.vstx - WWFC_BLOG_M" xr:uid="{5F9FF0E4-E1E7-4143-B2F6-A6277BB78C6B}"/>
+    <hyperlink ref="A151" r:id="rId150" location="WWFC_BLOG_R2L" display="WWFC_BLOG_R2L.vstx - WWFC_BLOG_R2L" xr:uid="{2F763571-FCB7-4AC6-9F7F-020DB2D31BD4}"/>
+    <hyperlink ref="A152" r:id="rId151" location="WWFC_CONTENTRICH_M" display="WWFC_CONTENTRICH_M.vstx - WWFC_CONTENTRICH_M" xr:uid="{682E6164-4882-48A2-AC61-0FF95FAA5F4D}"/>
+    <hyperlink ref="A153" r:id="rId152" location="WWFC_CONTENTRICH_R2L" display="WWFC_CONTENTRICH_R2L.vstx - WWFC_CONTENTRICH_R2L" xr:uid="{816A2BA9-B2BF-4D91-9540-651FDF4081E6}"/>
+    <hyperlink ref="A154" r:id="rId153" location="WWFC_ECOMMERCE_M" display="WWFC_ECOMMERCE_M.vstx - WWFC_ECOMMERCE_M" xr:uid="{9C8B8652-F3FF-44BB-9DD2-D21A90510F1D}"/>
+    <hyperlink ref="A155" r:id="rId154" location="WWFC_ECOMMERCE_R2L" display="WWFC_ECOMMERCE_R2L.vstx - WWFC_ECOMMERCE_R2L" xr:uid="{6B74A756-2683-4E50-9031-AF658552731B}"/>
+    <hyperlink ref="A156" r:id="rId155" location="WWFC_M" display="WWFC_M.vstx - WWFC_M" xr:uid="{F29F877B-FB1B-49B6-919D-D47C3ED23F49}"/>
+    <hyperlink ref="A157" r:id="rId156" location="XFUNC_M" display="XFUNC_M.vstx - XFUNC_M" xr:uid="{561EAB0C-30FF-4148-87F2-830DEAF58A4D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId157"/>

</xml_diff>